<commit_message>
Datos Pasados hasta el 28/06/21
</commit_message>
<xml_diff>
--- a/Gastos - Actualizado.xlsx
+++ b/Gastos - Actualizado.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Desktop\mis-gastos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,9 +23,158 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Setiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Turil</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Pendrive Mamá</t>
+  </si>
+  <si>
+    <t>Auris ZonaTecno Eli</t>
+  </si>
+  <si>
+    <t>TopTecnoUy (No tengo la menor idea)</t>
+  </si>
+  <si>
+    <t>Google Drive</t>
+  </si>
+  <si>
+    <t>Copiplan (Trading)</t>
+  </si>
+  <si>
+    <t>Microsoft Pomodoro App</t>
+  </si>
+  <si>
+    <t>Logitech MX Keys</t>
+  </si>
+  <si>
+    <t>Farmacia (Omega 3 y Glucosamina)</t>
+  </si>
+  <si>
+    <t>Heladería</t>
+  </si>
+  <si>
+    <t>Loi (No tengo la menor idea)</t>
+  </si>
+  <si>
+    <t>Lentes Ruglio</t>
+  </si>
+  <si>
+    <t>Oculista Ruglio</t>
+  </si>
+  <si>
+    <t>Farmacia (Omega 3)</t>
+  </si>
+  <si>
+    <t>Tratamiento Bruna (Pastillas y Comida)</t>
+  </si>
+  <si>
+    <t>Farmacia (Parches Ketofen)</t>
+  </si>
+  <si>
+    <t>El Clon</t>
+  </si>
+  <si>
+    <t>Española Resonancia</t>
+  </si>
+  <si>
+    <t>Española Sociedad</t>
+  </si>
+  <si>
+    <t>Loi (Camara y Accesorios)</t>
+  </si>
+  <si>
+    <t>MercadoPago (No tengo la menor idea)</t>
+  </si>
+  <si>
+    <t>Chorros de EQUITAL</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Spotify</t>
+  </si>
+  <si>
+    <t>Zonatecno EDIFIERs</t>
+  </si>
+  <si>
+    <t>Comida Bruna</t>
+  </si>
+  <si>
+    <t>Española Movil</t>
+  </si>
+  <si>
+    <t>SiSi Regalo Cristi</t>
+  </si>
+  <si>
+    <t>Sociedad Bruna</t>
+  </si>
+  <si>
+    <t>Twitch</t>
+  </si>
+  <si>
+    <t>Veterinaria Bruna Tratamiento</t>
+  </si>
+  <si>
+    <t>Toto Championes Deportivos</t>
+  </si>
+  <si>
+    <t>Sillas de Escritorio</t>
+  </si>
+  <si>
+    <t>Costo OCA</t>
+  </si>
+  <si>
+    <t>Uber</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,13 +182,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,8 +223,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +509,665 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="62.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>734</v>
+      </c>
+      <c r="C2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>225</v>
+      </c>
+      <c r="C4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>295</v>
+      </c>
+      <c r="C5">
+        <v>295</v>
+      </c>
+      <c r="D5">
+        <v>295</v>
+      </c>
+      <c r="E5">
+        <v>295</v>
+      </c>
+      <c r="F5">
+        <v>295</v>
+      </c>
+      <c r="G5">
+        <v>295</v>
+      </c>
+      <c r="H5">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>90</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>90</v>
+      </c>
+      <c r="F6">
+        <v>90</v>
+      </c>
+      <c r="G6">
+        <v>90</v>
+      </c>
+      <c r="H6">
+        <v>90</v>
+      </c>
+      <c r="I6">
+        <v>90</v>
+      </c>
+      <c r="J6">
+        <v>90</v>
+      </c>
+      <c r="K6">
+        <v>90</v>
+      </c>
+      <c r="L6">
+        <v>90</v>
+      </c>
+      <c r="M6">
+        <v>90</v>
+      </c>
+      <c r="N6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2">
+        <v>70</v>
+      </c>
+      <c r="C8" s="2">
+        <v>70</v>
+      </c>
+      <c r="D8" s="2">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2">
+        <v>70</v>
+      </c>
+      <c r="F8" s="2">
+        <v>70</v>
+      </c>
+      <c r="G8" s="2">
+        <v>70</v>
+      </c>
+      <c r="H8" s="2">
+        <v>70</v>
+      </c>
+      <c r="I8" s="2">
+        <v>70</v>
+      </c>
+      <c r="J8" s="2">
+        <v>70</v>
+      </c>
+      <c r="K8" s="2">
+        <v>70</v>
+      </c>
+      <c r="L8" s="2">
+        <v>70</v>
+      </c>
+      <c r="M8" s="2">
+        <v>70</v>
+      </c>
+      <c r="N8" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>511</v>
+      </c>
+      <c r="C9">
+        <v>511</v>
+      </c>
+      <c r="D9">
+        <v>511</v>
+      </c>
+      <c r="E9">
+        <v>511</v>
+      </c>
+      <c r="F9">
+        <v>511</v>
+      </c>
+      <c r="G9">
+        <v>511</v>
+      </c>
+      <c r="H9">
+        <v>511</v>
+      </c>
+      <c r="I9">
+        <v>511</v>
+      </c>
+      <c r="J9">
+        <v>511</v>
+      </c>
+      <c r="K9">
+        <v>511</v>
+      </c>
+      <c r="L9">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>186</v>
+      </c>
+      <c r="C12">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>565</v>
+      </c>
+      <c r="C13">
+        <v>565</v>
+      </c>
+      <c r="D13">
+        <v>565</v>
+      </c>
+      <c r="E13">
+        <v>565</v>
+      </c>
+      <c r="F13">
+        <v>565</v>
+      </c>
+      <c r="G13">
+        <v>565</v>
+      </c>
+      <c r="H13">
+        <v>565</v>
+      </c>
+      <c r="I13">
+        <v>565</v>
+      </c>
+      <c r="J13">
+        <v>565</v>
+      </c>
+      <c r="K13">
+        <v>565</v>
+      </c>
+      <c r="L13">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>500</v>
+      </c>
+      <c r="C14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>702</v>
+      </c>
+      <c r="C16">
+        <v>702</v>
+      </c>
+      <c r="D16">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>495</v>
+      </c>
+      <c r="C18">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>180</v>
+      </c>
+      <c r="C20">
+        <v>180</v>
+      </c>
+      <c r="D20">
+        <v>180</v>
+      </c>
+      <c r="E20">
+        <v>180</v>
+      </c>
+      <c r="F20">
+        <v>180</v>
+      </c>
+      <c r="G20">
+        <v>180</v>
+      </c>
+      <c r="H20">
+        <v>180</v>
+      </c>
+      <c r="I20">
+        <v>180</v>
+      </c>
+      <c r="J20">
+        <v>180</v>
+      </c>
+      <c r="K20">
+        <v>180</v>
+      </c>
+      <c r="L20">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>195</v>
+      </c>
+      <c r="C21">
+        <v>195</v>
+      </c>
+      <c r="D21">
+        <v>195</v>
+      </c>
+      <c r="E21">
+        <v>195</v>
+      </c>
+      <c r="F21">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>198</v>
+      </c>
+      <c r="C22">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2">
+        <v>326</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>600</v>
+      </c>
+      <c r="C24">
+        <v>600</v>
+      </c>
+      <c r="D24">
+        <v>600</v>
+      </c>
+      <c r="E24">
+        <v>600</v>
+      </c>
+      <c r="F24">
+        <v>600</v>
+      </c>
+      <c r="G24">
+        <v>600</v>
+      </c>
+      <c r="H24">
+        <v>600</v>
+      </c>
+      <c r="I24">
+        <v>600</v>
+      </c>
+      <c r="J24">
+        <v>600</v>
+      </c>
+      <c r="K24">
+        <v>600</v>
+      </c>
+      <c r="L24">
+        <v>600</v>
+      </c>
+      <c r="M24">
+        <v>600</v>
+      </c>
+      <c r="N24">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25">
+        <v>400</v>
+      </c>
+      <c r="C25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>295</v>
+      </c>
+      <c r="C26">
+        <v>295</v>
+      </c>
+      <c r="D26">
+        <v>295</v>
+      </c>
+      <c r="E26">
+        <v>295</v>
+      </c>
+      <c r="F26">
+        <v>295</v>
+      </c>
+      <c r="G26">
+        <v>295</v>
+      </c>
+      <c r="H26">
+        <v>295</v>
+      </c>
+      <c r="I26">
+        <v>295</v>
+      </c>
+      <c r="J26">
+        <v>295</v>
+      </c>
+      <c r="K26">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
+        <v>1431</v>
+      </c>
+      <c r="C27">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
+        <v>931</v>
+      </c>
+      <c r="C33">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34">
+        <v>450</v>
+      </c>
+      <c r="C34">
+        <v>450</v>
+      </c>
+      <c r="D34">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>1100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gastos Totales Generales calculados
</commit_message>
<xml_diff>
--- a/Gastos - Actualizado.xlsx
+++ b/Gastos - Actualizado.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$N$40</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Julio</t>
   </si>
@@ -168,13 +171,52 @@
   </si>
   <si>
     <t>Uber</t>
+  </si>
+  <si>
+    <t>Tritofano + Magnesio + B6</t>
+  </si>
+  <si>
+    <t>STM</t>
+  </si>
+  <si>
+    <t>TOTAL OCA</t>
+  </si>
+  <si>
+    <t>Gastos Comunes</t>
+  </si>
+  <si>
+    <t>Impuesto a la Puerta</t>
+  </si>
+  <si>
+    <t>Antel</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>OCA</t>
+  </si>
+  <si>
+    <t>Gastos Fijos</t>
+  </si>
+  <si>
+    <t>Alimentación</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>TOTAL GASTOS FIJOS</t>
+  </si>
+  <si>
+    <t>TOTAL GENERAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,8 +232,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +267,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -223,12 +292,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,376 +644,410 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>734</v>
-      </c>
-      <c r="C2">
-        <v>367</v>
-      </c>
+      <c r="A2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>543</v>
+        <v>734</v>
+      </c>
+      <c r="C3">
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>225</v>
-      </c>
-      <c r="C4">
-        <v>225</v>
+        <v>543</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>295</v>
+        <v>225</v>
       </c>
       <c r="C5">
-        <v>295</v>
-      </c>
-      <c r="D5">
-        <v>295</v>
-      </c>
-      <c r="E5">
-        <v>295</v>
-      </c>
-      <c r="F5">
-        <v>295</v>
-      </c>
-      <c r="G5">
-        <v>295</v>
-      </c>
-      <c r="H5">
-        <v>295</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>295</v>
       </c>
       <c r="C6">
-        <v>90</v>
+        <v>295</v>
       </c>
       <c r="D6">
-        <v>90</v>
+        <v>295</v>
       </c>
       <c r="E6">
-        <v>90</v>
+        <v>295</v>
       </c>
       <c r="F6">
-        <v>90</v>
+        <v>295</v>
       </c>
       <c r="G6">
-        <v>90</v>
+        <v>295</v>
       </c>
       <c r="H6">
-        <v>90</v>
-      </c>
-      <c r="I6">
-        <v>90</v>
-      </c>
-      <c r="J6">
-        <v>90</v>
-      </c>
-      <c r="K6">
-        <v>90</v>
-      </c>
-      <c r="L6">
-        <v>90</v>
-      </c>
-      <c r="M6">
-        <v>90</v>
-      </c>
-      <c r="N6">
-        <v>90</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+      <c r="C7">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>90</v>
+      </c>
+      <c r="E7">
+        <v>90</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <v>90</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7">
+        <v>90</v>
+      </c>
+      <c r="J7">
+        <v>90</v>
+      </c>
+      <c r="K7">
+        <v>90</v>
+      </c>
+      <c r="L7">
+        <v>90</v>
+      </c>
+      <c r="M7">
+        <v>90</v>
+      </c>
+      <c r="N7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>70</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>70</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>70</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>70</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>70</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <v>70</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <v>70</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I9" s="2">
         <v>70</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J9" s="2">
         <v>70</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K9" s="2">
         <v>70</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L9" s="2">
         <v>70</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M9" s="2">
         <v>70</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N9" s="2">
         <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>511</v>
-      </c>
-      <c r="C9">
-        <v>511</v>
-      </c>
-      <c r="D9">
-        <v>511</v>
-      </c>
-      <c r="E9">
-        <v>511</v>
-      </c>
-      <c r="F9">
-        <v>511</v>
-      </c>
-      <c r="G9">
-        <v>511</v>
-      </c>
-      <c r="H9">
-        <v>511</v>
-      </c>
-      <c r="I9">
-        <v>511</v>
-      </c>
-      <c r="J9">
-        <v>511</v>
-      </c>
-      <c r="K9">
-        <v>511</v>
-      </c>
-      <c r="L9">
-        <v>511</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>1640</v>
+        <v>511</v>
+      </c>
+      <c r="C10">
+        <v>511</v>
+      </c>
+      <c r="D10">
+        <v>511</v>
+      </c>
+      <c r="E10">
+        <v>511</v>
+      </c>
+      <c r="F10">
+        <v>511</v>
+      </c>
+      <c r="G10">
+        <v>511</v>
+      </c>
+      <c r="H10">
+        <v>511</v>
+      </c>
+      <c r="I10">
+        <v>511</v>
+      </c>
+      <c r="J10">
+        <v>511</v>
+      </c>
+      <c r="K10">
+        <v>511</v>
+      </c>
+      <c r="L10">
+        <v>511</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11">
-        <v>440</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12">
-        <v>186</v>
-      </c>
-      <c r="C12">
-        <v>186</v>
+        <v>440</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13">
-        <v>565</v>
+        <v>186</v>
       </c>
       <c r="C13">
-        <v>565</v>
-      </c>
-      <c r="D13">
-        <v>565</v>
-      </c>
-      <c r="E13">
-        <v>565</v>
-      </c>
-      <c r="F13">
-        <v>565</v>
-      </c>
-      <c r="G13">
-        <v>565</v>
-      </c>
-      <c r="H13">
-        <v>565</v>
-      </c>
-      <c r="I13">
-        <v>565</v>
-      </c>
-      <c r="J13">
-        <v>565</v>
-      </c>
-      <c r="K13">
-        <v>565</v>
-      </c>
-      <c r="L13">
-        <v>565</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14">
-        <v>500</v>
+        <v>565</v>
       </c>
       <c r="C14">
-        <v>500</v>
+        <v>565</v>
+      </c>
+      <c r="D14">
+        <v>565</v>
+      </c>
+      <c r="E14">
+        <v>565</v>
+      </c>
+      <c r="F14">
+        <v>565</v>
+      </c>
+      <c r="G14">
+        <v>565</v>
+      </c>
+      <c r="H14">
+        <v>565</v>
+      </c>
+      <c r="I14">
+        <v>565</v>
+      </c>
+      <c r="J14">
+        <v>565</v>
+      </c>
+      <c r="K14">
+        <v>565</v>
+      </c>
+      <c r="L14">
+        <v>565</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15">
-        <v>786</v>
+        <v>500</v>
+      </c>
+      <c r="C15">
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16">
-        <v>702</v>
-      </c>
-      <c r="C16">
-        <v>702</v>
-      </c>
-      <c r="D16">
-        <v>702</v>
+        <v>786</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17">
-        <v>1287</v>
+        <v>702</v>
+      </c>
+      <c r="C17">
+        <v>702</v>
+      </c>
+      <c r="D17">
+        <v>702</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18">
-        <v>495</v>
-      </c>
-      <c r="C18">
-        <v>495</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19">
-        <v>674</v>
+        <v>495</v>
+      </c>
+      <c r="C19">
+        <v>495</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="C20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="D20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="E20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="F20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="G20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="H20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="I20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="J20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="K20">
-        <v>180</v>
+        <v>674</v>
       </c>
       <c r="L20">
-        <v>180</v>
+        <v>674</v>
+      </c>
+      <c r="M20">
+        <v>674</v>
+      </c>
+      <c r="N20">
+        <v>674</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="C21">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D21">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E21">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="F21">
-        <v>195</v>
+        <v>180</v>
+      </c>
+      <c r="G21">
+        <v>180</v>
+      </c>
+      <c r="H21">
+        <v>180</v>
+      </c>
+      <c r="I21">
+        <v>180</v>
+      </c>
+      <c r="J21">
+        <v>180</v>
+      </c>
+      <c r="K21">
+        <v>180</v>
+      </c>
+      <c r="L21">
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -942,228 +1055,847 @@
         <v>33</v>
       </c>
       <c r="B22">
+        <v>195</v>
+      </c>
+      <c r="C22">
+        <v>195</v>
+      </c>
+      <c r="D22">
+        <v>195</v>
+      </c>
+      <c r="E22">
+        <v>195</v>
+      </c>
+      <c r="F22">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
         <v>198</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>326</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24">
-        <v>600</v>
-      </c>
-      <c r="C24">
-        <v>600</v>
-      </c>
-      <c r="D24">
-        <v>600</v>
-      </c>
-      <c r="E24">
-        <v>600</v>
-      </c>
-      <c r="F24">
-        <v>600</v>
-      </c>
-      <c r="G24">
-        <v>600</v>
-      </c>
-      <c r="H24">
-        <v>600</v>
-      </c>
-      <c r="I24">
-        <v>600</v>
-      </c>
-      <c r="J24">
-        <v>600</v>
-      </c>
-      <c r="K24">
-        <v>600</v>
-      </c>
-      <c r="L24">
-        <v>600</v>
-      </c>
-      <c r="M24">
-        <v>600</v>
-      </c>
-      <c r="N24">
-        <v>600</v>
-      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="C25">
-        <v>400</v>
+        <v>600</v>
+      </c>
+      <c r="D25">
+        <v>600</v>
+      </c>
+      <c r="E25">
+        <v>600</v>
+      </c>
+      <c r="F25">
+        <v>600</v>
+      </c>
+      <c r="G25">
+        <v>600</v>
+      </c>
+      <c r="H25">
+        <v>600</v>
+      </c>
+      <c r="I25">
+        <v>600</v>
+      </c>
+      <c r="J25">
+        <v>600</v>
+      </c>
+      <c r="K25">
+        <v>600</v>
+      </c>
+      <c r="L25">
+        <v>600</v>
+      </c>
+      <c r="M25">
+        <v>600</v>
+      </c>
+      <c r="N25">
+        <v>600</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26">
-        <v>295</v>
+        <v>400</v>
       </c>
       <c r="C26">
-        <v>295</v>
-      </c>
-      <c r="D26">
-        <v>295</v>
-      </c>
-      <c r="E26">
-        <v>295</v>
-      </c>
-      <c r="F26">
-        <v>295</v>
-      </c>
-      <c r="G26">
-        <v>295</v>
-      </c>
-      <c r="H26">
-        <v>295</v>
-      </c>
-      <c r="I26">
-        <v>295</v>
-      </c>
-      <c r="J26">
-        <v>295</v>
-      </c>
-      <c r="K26">
-        <v>295</v>
+        <v>400</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27">
-        <v>1431</v>
+        <v>295</v>
       </c>
       <c r="C27">
-        <v>1431</v>
+        <v>295</v>
+      </c>
+      <c r="D27">
+        <v>295</v>
+      </c>
+      <c r="E27">
+        <v>295</v>
+      </c>
+      <c r="F27">
+        <v>295</v>
+      </c>
+      <c r="G27">
+        <v>295</v>
+      </c>
+      <c r="H27">
+        <v>295</v>
+      </c>
+      <c r="I27">
+        <v>295</v>
+      </c>
+      <c r="J27">
+        <v>295</v>
+      </c>
+      <c r="K27">
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28">
-        <v>783</v>
+        <v>1431</v>
+      </c>
+      <c r="C28">
+        <v>1431</v>
+      </c>
+      <c r="D28">
+        <v>1431</v>
+      </c>
+      <c r="E28">
+        <v>1431</v>
+      </c>
+      <c r="F28">
+        <v>1431</v>
+      </c>
+      <c r="G28">
+        <v>1431</v>
+      </c>
+      <c r="H28">
+        <v>1431</v>
+      </c>
+      <c r="I28">
+        <v>1431</v>
+      </c>
+      <c r="J28">
+        <v>1431</v>
+      </c>
+      <c r="K28">
+        <v>1431</v>
+      </c>
+      <c r="L28">
+        <v>1431</v>
+      </c>
+      <c r="M28">
+        <v>1431</v>
+      </c>
+      <c r="N28">
+        <v>1431</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29">
-        <v>357</v>
+        <v>783</v>
+      </c>
+      <c r="C29">
+        <v>783</v>
+      </c>
+      <c r="D29">
+        <v>783</v>
+      </c>
+      <c r="E29">
+        <v>783</v>
+      </c>
+      <c r="F29">
+        <v>783</v>
+      </c>
+      <c r="G29">
+        <v>783</v>
+      </c>
+      <c r="H29">
+        <v>783</v>
+      </c>
+      <c r="I29">
+        <v>783</v>
+      </c>
+      <c r="J29">
+        <v>783</v>
+      </c>
+      <c r="K29">
+        <v>783</v>
+      </c>
+      <c r="L29">
+        <v>783</v>
+      </c>
+      <c r="M29">
+        <v>783</v>
+      </c>
+      <c r="N29">
+        <v>783</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B30">
-        <v>869</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B31">
-        <v>380</v>
+        <v>869</v>
+      </c>
+      <c r="D31">
+        <v>870</v>
+      </c>
+      <c r="F31">
+        <v>870</v>
+      </c>
+      <c r="H31">
+        <v>870</v>
+      </c>
+      <c r="J31">
+        <v>870</v>
+      </c>
+      <c r="L31">
+        <v>870</v>
+      </c>
+      <c r="N31">
+        <v>870</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32">
+        <v>1250</v>
+      </c>
+      <c r="E32">
+        <v>1250</v>
+      </c>
+      <c r="G32">
+        <v>1250</v>
+      </c>
+      <c r="I32">
+        <v>1250</v>
+      </c>
+      <c r="K32">
+        <v>1250</v>
+      </c>
+      <c r="M32">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>42</v>
       </c>
-      <c r="B32">
+      <c r="B34">
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>43</v>
       </c>
-      <c r="B33">
+      <c r="B35">
         <v>931</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <v>931</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
-      <c r="B34">
+      <c r="B36">
         <v>450</v>
       </c>
-      <c r="C34">
+      <c r="C36">
         <v>450</v>
       </c>
-      <c r="D34">
+      <c r="D36">
         <v>450</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>45</v>
       </c>
-      <c r="B35">
+      <c r="B37">
         <v>750</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>23</v>
       </c>
-      <c r="B36">
+      <c r="B38">
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>46</v>
       </c>
-      <c r="B37">
+      <c r="B39">
         <v>450</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>47</v>
       </c>
-      <c r="B38">
+      <c r="B40">
         <v>1100</v>
+      </c>
+      <c r="C40">
+        <v>1000</v>
+      </c>
+      <c r="D40">
+        <v>1000</v>
+      </c>
+      <c r="E40">
+        <v>1000</v>
+      </c>
+      <c r="F40">
+        <v>1000</v>
+      </c>
+      <c r="G40">
+        <v>1000</v>
+      </c>
+      <c r="H40">
+        <v>1000</v>
+      </c>
+      <c r="I40">
+        <v>1000</v>
+      </c>
+      <c r="J40">
+        <v>1000</v>
+      </c>
+      <c r="K40">
+        <v>1000</v>
+      </c>
+      <c r="L40">
+        <v>1000</v>
+      </c>
+      <c r="M40">
+        <v>1000</v>
+      </c>
+      <c r="N40">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="3">
+        <f>SUM(B3:B46)</f>
+        <v>20435</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" ref="C47:N47" si="0">SUM(C3:C46)</f>
+        <v>12393</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="0"/>
+        <v>8711</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="0"/>
+        <v>7939</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="0"/>
+        <v>7559</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" si="0"/>
+        <v>7744</v>
+      </c>
+      <c r="H47" s="3">
+        <f t="shared" si="0"/>
+        <v>7364</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="0"/>
+        <v>7449</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="0"/>
+        <v>7069</v>
+      </c>
+      <c r="K47" s="3">
+        <f t="shared" si="0"/>
+        <v>7449</v>
+      </c>
+      <c r="L47" s="3">
+        <f t="shared" si="0"/>
+        <v>6774</v>
+      </c>
+      <c r="M47" s="3">
+        <f t="shared" si="0"/>
+        <v>5898</v>
+      </c>
+      <c r="N47" s="3">
+        <f t="shared" si="0"/>
+        <v>5518</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>2320</v>
+      </c>
+      <c r="C49">
+        <v>2320</v>
+      </c>
+      <c r="D49">
+        <v>2320</v>
+      </c>
+      <c r="E49">
+        <v>2320</v>
+      </c>
+      <c r="F49">
+        <v>2320</v>
+      </c>
+      <c r="G49">
+        <v>2320</v>
+      </c>
+      <c r="H49">
+        <v>2320</v>
+      </c>
+      <c r="I49">
+        <v>2320</v>
+      </c>
+      <c r="J49">
+        <v>2320</v>
+      </c>
+      <c r="K49">
+        <v>2320</v>
+      </c>
+      <c r="L49">
+        <v>2320</v>
+      </c>
+      <c r="M49">
+        <v>2320</v>
+      </c>
+      <c r="N49">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <v>1200</v>
+      </c>
+      <c r="D50">
+        <v>1200</v>
+      </c>
+      <c r="F50">
+        <v>1200</v>
+      </c>
+      <c r="H50">
+        <v>1200</v>
+      </c>
+      <c r="J50">
+        <v>1200</v>
+      </c>
+      <c r="L50">
+        <v>1200</v>
+      </c>
+      <c r="N50">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51">
+        <v>1700</v>
+      </c>
+      <c r="C51">
+        <v>1700</v>
+      </c>
+      <c r="D51">
+        <v>1700</v>
+      </c>
+      <c r="E51">
+        <v>1700</v>
+      </c>
+      <c r="F51">
+        <v>1700</v>
+      </c>
+      <c r="G51">
+        <v>1700</v>
+      </c>
+      <c r="H51">
+        <v>1700</v>
+      </c>
+      <c r="I51">
+        <v>1700</v>
+      </c>
+      <c r="J51">
+        <v>1700</v>
+      </c>
+      <c r="K51">
+        <v>1700</v>
+      </c>
+      <c r="L51">
+        <v>1700</v>
+      </c>
+      <c r="M51">
+        <v>1700</v>
+      </c>
+      <c r="N51">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52">
+        <v>3000</v>
+      </c>
+      <c r="C52">
+        <v>4000</v>
+      </c>
+      <c r="D52">
+        <v>3500</v>
+      </c>
+      <c r="E52">
+        <v>2000</v>
+      </c>
+      <c r="F52">
+        <v>2000</v>
+      </c>
+      <c r="G52">
+        <v>2000</v>
+      </c>
+      <c r="H52">
+        <v>2000</v>
+      </c>
+      <c r="I52">
+        <v>2000</v>
+      </c>
+      <c r="J52">
+        <v>2000</v>
+      </c>
+      <c r="K52">
+        <v>2000</v>
+      </c>
+      <c r="L52">
+        <v>2000</v>
+      </c>
+      <c r="M52">
+        <v>2000</v>
+      </c>
+      <c r="N52">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="3">
+        <f>SUM(B49:B52)</f>
+        <v>8220</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" ref="C53:N53" si="1">SUM(C49:C52)</f>
+        <v>8020</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="1"/>
+        <v>8720</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="1"/>
+        <v>6020</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="1"/>
+        <v>7220</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="1"/>
+        <v>6020</v>
+      </c>
+      <c r="H53" s="3">
+        <f t="shared" si="1"/>
+        <v>7220</v>
+      </c>
+      <c r="I53" s="3">
+        <f t="shared" si="1"/>
+        <v>6020</v>
+      </c>
+      <c r="J53" s="3">
+        <f t="shared" si="1"/>
+        <v>7220</v>
+      </c>
+      <c r="K53" s="3">
+        <f t="shared" si="1"/>
+        <v>6020</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="1"/>
+        <v>7220</v>
+      </c>
+      <c r="M53" s="3">
+        <f t="shared" si="1"/>
+        <v>6020</v>
+      </c>
+      <c r="N53" s="3">
+        <f t="shared" si="1"/>
+        <v>7220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55">
+        <v>10000</v>
+      </c>
+      <c r="C55">
+        <v>10000</v>
+      </c>
+      <c r="D55">
+        <v>10000</v>
+      </c>
+      <c r="E55">
+        <v>10000</v>
+      </c>
+      <c r="F55">
+        <v>10000</v>
+      </c>
+      <c r="G55">
+        <v>10000</v>
+      </c>
+      <c r="H55">
+        <v>10000</v>
+      </c>
+      <c r="I55">
+        <v>10000</v>
+      </c>
+      <c r="J55">
+        <v>10000</v>
+      </c>
+      <c r="K55">
+        <v>10000</v>
+      </c>
+      <c r="L55">
+        <v>10000</v>
+      </c>
+      <c r="M55">
+        <v>10000</v>
+      </c>
+      <c r="N55">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="7">
+        <f>SUM(B47+B53+B55)</f>
+        <v>38655</v>
+      </c>
+      <c r="C58" s="7">
+        <f t="shared" ref="C58:N58" si="2">SUM(C47+C53+C55)</f>
+        <v>30413</v>
+      </c>
+      <c r="D58" s="7">
+        <f t="shared" si="2"/>
+        <v>27431</v>
+      </c>
+      <c r="E58" s="7">
+        <f t="shared" si="2"/>
+        <v>23959</v>
+      </c>
+      <c r="F58" s="7">
+        <f t="shared" si="2"/>
+        <v>24779</v>
+      </c>
+      <c r="G58" s="7">
+        <f t="shared" si="2"/>
+        <v>23764</v>
+      </c>
+      <c r="H58" s="7">
+        <f t="shared" si="2"/>
+        <v>24584</v>
+      </c>
+      <c r="I58" s="7">
+        <f t="shared" si="2"/>
+        <v>23469</v>
+      </c>
+      <c r="J58" s="7">
+        <f t="shared" si="2"/>
+        <v>24289</v>
+      </c>
+      <c r="K58" s="7">
+        <f t="shared" si="2"/>
+        <v>23469</v>
+      </c>
+      <c r="L58" s="7">
+        <f t="shared" si="2"/>
+        <v>23994</v>
+      </c>
+      <c r="M58" s="7">
+        <f t="shared" si="2"/>
+        <v>21918</v>
+      </c>
+      <c r="N58" s="7">
+        <f t="shared" si="2"/>
+        <v>22738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>